<commit_message>
Update tracking on 29/05/2012
</commit_message>
<xml_diff>
--- a/Document/Plan/OPMS_Plan Tracking.xlsx
+++ b/Document/Plan/OPMS_Plan Tracking.xlsx
@@ -308,6 +308,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -320,8 +322,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -621,7 +621,7 @@
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
       <pane ySplit="840" activePane="bottomLeft"/>
       <selection activeCell="E2" sqref="E1:E1048576"/>
-      <selection pane="bottomLeft" activeCell="C12" sqref="C12"/>
+      <selection pane="bottomLeft" activeCell="P14" sqref="P14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -654,52 +654,52 @@
       <c r="E1" t="s">
         <v>73</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3" t="s">
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3"/>
-      <c r="O1" s="3" t="s">
+      <c r="L1" s="5"/>
+      <c r="M1" s="5"/>
+      <c r="N1" s="5"/>
+      <c r="O1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="P1" s="3"/>
-      <c r="Q1" s="3"/>
-      <c r="R1" s="3"/>
-      <c r="S1" s="3" t="s">
+      <c r="P1" s="5"/>
+      <c r="Q1" s="5"/>
+      <c r="R1" s="5"/>
+      <c r="S1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="T1" s="3"/>
-      <c r="U1" s="3"/>
-      <c r="V1" s="3"/>
-      <c r="W1" s="4">
+      <c r="T1" s="5"/>
+      <c r="U1" s="5"/>
+      <c r="V1" s="5"/>
+      <c r="W1" s="6">
         <v>40974</v>
       </c>
-      <c r="X1" s="5"/>
-      <c r="Y1" s="5"/>
-      <c r="Z1" s="5"/>
-      <c r="AA1" s="2">
+      <c r="X1" s="7"/>
+      <c r="Y1" s="7"/>
+      <c r="Z1" s="7"/>
+      <c r="AA1" s="4">
         <v>41035</v>
       </c>
-      <c r="AB1" s="2"/>
-      <c r="AC1" s="2"/>
-      <c r="AD1" s="2"/>
-      <c r="AE1" s="2">
+      <c r="AB1" s="4"/>
+      <c r="AC1" s="4"/>
+      <c r="AD1" s="4"/>
+      <c r="AE1" s="4">
         <v>41096</v>
       </c>
-      <c r="AF1" s="2"/>
-      <c r="AG1" s="2"/>
-      <c r="AH1" s="2"/>
-      <c r="AI1" s="3"/>
-      <c r="AJ1" s="3"/>
-      <c r="AK1" s="3"/>
-      <c r="AL1" s="3"/>
+      <c r="AF1" s="4"/>
+      <c r="AG1" s="4"/>
+      <c r="AH1" s="4"/>
+      <c r="AI1" s="5"/>
+      <c r="AJ1" s="5"/>
+      <c r="AK1" s="5"/>
+      <c r="AL1" s="5"/>
     </row>
     <row r="2" spans="1:38">
       <c r="E2" t="s">
@@ -822,10 +822,10 @@
       <c r="D5" t="s">
         <v>17</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="F5" s="7" t="s">
+      <c r="F5" s="3" t="s">
         <v>77</v>
       </c>
       <c r="K5">
@@ -851,10 +851,10 @@
       <c r="D6" t="s">
         <v>17</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="E6" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="F6" s="7" t="s">
+      <c r="F6" s="3" t="s">
         <v>79</v>
       </c>
       <c r="K6">
@@ -880,10 +880,10 @@
       <c r="D7" t="s">
         <v>17</v>
       </c>
-      <c r="E7" s="7" t="s">
+      <c r="E7" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="F7" s="7" t="s">
+      <c r="F7" s="3" t="s">
         <v>81</v>
       </c>
       <c r="K7">
@@ -946,7 +946,7 @@
       <c r="D10" t="s">
         <v>17</v>
       </c>
-      <c r="E10" s="7"/>
+      <c r="E10" s="3"/>
       <c r="L10">
         <v>50</v>
       </c>
@@ -956,12 +956,16 @@
       <c r="N10">
         <v>400</v>
       </c>
+      <c r="O10">
+        <f>39+35+5</f>
+        <v>79</v>
+      </c>
       <c r="P10">
         <v>250</v>
       </c>
       <c r="Q10">
         <f>M10+O10</f>
-        <v>18</v>
+        <v>97</v>
       </c>
       <c r="R10">
         <v>400</v>
@@ -971,7 +975,7 @@
       </c>
       <c r="U10">
         <f>Q10+S10</f>
-        <v>18</v>
+        <v>97</v>
       </c>
       <c r="V10">
         <v>400</v>
@@ -981,7 +985,7 @@
       </c>
       <c r="Y10">
         <f>U10+W10</f>
-        <v>18</v>
+        <v>97</v>
       </c>
       <c r="Z10">
         <v>400</v>

</xml_diff>